<commit_message>
feat: Add 'title' field to product model and enhance import, search, and display functionalities across various components.
</commit_message>
<xml_diff>
--- a/public/product-import-template.xlsx
+++ b/public/product-import-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitul\Herd\product-portal\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F207A7-7367-4612-BFF7-CCAE51B041C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C44C953-FB7C-4802-B03D-31CA063DC01D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Generators" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="56">
   <si>
     <t>Hold</t>
   </si>
@@ -188,6 +188,9 @@
   </si>
   <si>
     <t>Kw</t>
+  </si>
+  <si>
+    <t>Title</t>
   </si>
 </sst>
 </file>
@@ -544,7 +547,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+    <sheetView topLeftCell="V1" workbookViewId="0">
       <selection activeCell="AP1" sqref="AP1"/>
     </sheetView>
   </sheetViews>
@@ -958,10 +961,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:L1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -978,7 +981,7 @@
     <col min="12" max="12" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1014,6 +1017,9 @@
       </c>
       <c r="L1" s="1" t="s">
         <v>37</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>